<commit_message>
Applied browser selection logic in DataEngine
</commit_message>
<xml_diff>
--- a/bin/dataEngine/DataEngine.xlsx
+++ b/bin/dataEngine/DataEngine.xlsx
@@ -12,17 +12,19 @@
     <sheet name="PageObjectModel" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="ActionKeywords">PageObjectModel!$D$2:$D$26</definedName>
+    <definedName name="ActionKeywords">PageObjectModel!$F$2:$F$26</definedName>
+    <definedName name="CartPage">PageObjectModel!$E$2:$E$10</definedName>
     <definedName name="HomePage">PageObjectModel!$B$2:$B$10</definedName>
     <definedName name="LoginPage">PageObjectModel!$C$2:$C$10</definedName>
     <definedName name="PageName">PageObjectModel!$A$2:$A$10</definedName>
+    <definedName name="ShoppingPage">PageObjectModel!$D$2:$D$10</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="86">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -228,7 +230,58 @@
     <t>Test_Step_Description</t>
   </si>
   <si>
+    <t>ShoppingPage</t>
+  </si>
+  <si>
+    <t>CartPage</t>
+  </si>
+  <si>
+    <t>Shopping Page Objects</t>
+  </si>
+  <si>
+    <t>Cart Page Objects</t>
+  </si>
+  <si>
+    <t>lnk_ProductCategory</t>
+  </si>
+  <si>
+    <t>lnk_iPhones</t>
+  </si>
+  <si>
+    <t>btn_AddToCart</t>
+  </si>
+  <si>
+    <t>lbl_CurrentPrice</t>
+  </si>
+  <si>
+    <t>btn_GoToCheckOut</t>
+  </si>
+  <si>
+    <t>lbl_Checkout</t>
+  </si>
+  <si>
+    <t>btn_Continue</t>
+  </si>
+  <si>
+    <t>lnk_Product</t>
+  </si>
+  <si>
+    <t>txtbx_Qty</t>
+  </si>
+  <si>
+    <t>lbl_SubTotal</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -1162,9 +1215,7 @@
   <sheetPr codeName="Blad2"/>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1196,10 +1247,7 @@
         <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1213,7 +1261,7 @@
         <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1223,7 +1271,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>PageObjectModel!$E$2:$E$3</xm:f>
+            <xm:f>PageObjectModel!$G$2:$G$3</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C17</xm:sqref>
         </x14:dataValidation>
@@ -1239,7 +1287,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1293,9 +1341,11 @@
       <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="H2" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1315,7 +1365,7 @@
       </c>
       <c r="G3" s="4"/>
       <c r="H3" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1339,7 +1389,7 @@
       </c>
       <c r="G4" s="4"/>
       <c r="H4" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1365,7 +1415,7 @@
         <v>33</v>
       </c>
       <c r="H5" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1391,7 +1441,7 @@
         <v>34</v>
       </c>
       <c r="H6" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1415,7 +1465,7 @@
       </c>
       <c r="G7" s="4"/>
       <c r="H7" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1435,7 +1485,7 @@
       </c>
       <c r="G8" s="4"/>
       <c r="H8" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1459,7 +1509,7 @@
       </c>
       <c r="G9" s="4"/>
       <c r="H9" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1479,7 +1529,7 @@
       </c>
       <c r="G10" s="4"/>
       <c r="H10" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1497,9 +1547,11 @@
       <c r="F11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="H11" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1518,9 +1570,6 @@
         <v>5</v>
       </c>
       <c r="G12" s="3"/>
-      <c r="H12" t="s">
-        <v>68</v>
-      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -1542,9 +1591,6 @@
         <v>31</v>
       </c>
       <c r="G13" s="3"/>
-      <c r="H13" t="s">
-        <v>68</v>
-      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -1568,9 +1614,6 @@
       <c r="G14" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H14" t="s">
-        <v>68</v>
-      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -1594,9 +1637,6 @@
       <c r="G15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H15" t="s">
-        <v>68</v>
-      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -1618,11 +1658,8 @@
         <v>31</v>
       </c>
       <c r="G16" s="3"/>
-      <c r="H16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
@@ -1638,11 +1675,8 @@
         <v>6</v>
       </c>
       <c r="G17" s="3"/>
-      <c r="H17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>36</v>
       </c>
@@ -1664,11 +1698,8 @@
       <c r="G18" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>36</v>
       </c>
@@ -1684,9 +1715,6 @@
         <v>7</v>
       </c>
       <c r="G19" s="3"/>
-      <c r="H19" t="s">
-        <v>68</v>
-      </c>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -1707,22 +1735,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="18.7109375" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="27.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>58</v>
       </c>
@@ -1732,14 +1762,20 @@
       <c r="C1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>59</v>
       </c>
@@ -1749,14 +1785,20 @@
       <c r="C2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>60</v>
       </c>
@@ -1766,79 +1808,115 @@
       <c r="C3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>69</v>
+      </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="G10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Add to cart TC steps
</commit_message>
<xml_diff>
--- a/bin/dataEngine/DataEngine.xlsx
+++ b/bin/dataEngine/DataEngine.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="111">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -282,6 +282,81 @@
   </si>
   <si>
     <t>FAIL</t>
+  </si>
+  <si>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t>Add a product to cart</t>
+  </si>
+  <si>
+    <t>TC003_01</t>
+  </si>
+  <si>
+    <t>Click on Product Category</t>
+  </si>
+  <si>
+    <t>Click on iPhones</t>
+  </si>
+  <si>
+    <t>Verify and store product price</t>
+  </si>
+  <si>
+    <t>Add product to Cart</t>
+  </si>
+  <si>
+    <t>Navigate to Cart</t>
+  </si>
+  <si>
+    <t>TC004</t>
+  </si>
+  <si>
+    <t>TC003_02</t>
+  </si>
+  <si>
+    <t>TC003_03</t>
+  </si>
+  <si>
+    <t>TC003_04</t>
+  </si>
+  <si>
+    <t>TC003_05</t>
+  </si>
+  <si>
+    <t>TC003_06</t>
+  </si>
+  <si>
+    <t>TC003_07</t>
+  </si>
+  <si>
+    <t>TC003_08</t>
+  </si>
+  <si>
+    <t>TC003_09</t>
+  </si>
+  <si>
+    <t>TC003_10</t>
+  </si>
+  <si>
+    <t>TC003_11</t>
+  </si>
+  <si>
+    <t>TC003_12</t>
+  </si>
+  <si>
+    <t>TC003_13</t>
+  </si>
+  <si>
+    <t>TC003_14</t>
+  </si>
+  <si>
+    <t>Verify quantity of the product</t>
+  </si>
+  <si>
+    <t>Verify price of the product</t>
+  </si>
+  <si>
+    <t>storeValue</t>
   </si>
 </sst>
 </file>
@@ -1213,16 +1288,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Blad2"/>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="56.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="56.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1258,10 +1335,18 @@
         <v>37</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="D3" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1284,20 +1369,20 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Blad1"/>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="30.5703125" collapsed="true"/>
-    <col min="4" max="6" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="6" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1716,15 +1801,303 @@
       </c>
       <c r="G19" s="3"/>
     </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G29" s="4"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G33" s="4"/>
+    </row>
   </sheetData>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D19">
       <formula1>PageName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E33">
       <formula1>INDIRECT(D2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F33">
       <formula1>ActionKeywords</formula1>
     </dataValidation>
   </dataValidations>
@@ -1735,21 +2108,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="27.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1918,6 +2291,11 @@
       </c>
       <c r="G10" s="2"/>
     </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Extent Reporting feature
</commit_message>
<xml_diff>
--- a/bin/dataEngine/DataEngine.xlsx
+++ b/bin/dataEngine/DataEngine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="11295" windowHeight="8130"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="11295" windowHeight="8130" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="113">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -275,88 +275,94 @@
     <t>chrome</t>
   </si>
   <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t>Add a product to cart</t>
+  </si>
+  <si>
+    <t>TC003_01</t>
+  </si>
+  <si>
+    <t>Click on Product Category</t>
+  </si>
+  <si>
+    <t>Click on iPhones</t>
+  </si>
+  <si>
+    <t>Verify and store product price</t>
+  </si>
+  <si>
+    <t>Add product to Cart</t>
+  </si>
+  <si>
+    <t>Navigate to Cart</t>
+  </si>
+  <si>
+    <t>TC004</t>
+  </si>
+  <si>
+    <t>TC003_02</t>
+  </si>
+  <si>
+    <t>TC003_03</t>
+  </si>
+  <si>
+    <t>TC003_04</t>
+  </si>
+  <si>
+    <t>TC003_05</t>
+  </si>
+  <si>
+    <t>TC003_06</t>
+  </si>
+  <si>
+    <t>TC003_07</t>
+  </si>
+  <si>
+    <t>TC003_08</t>
+  </si>
+  <si>
+    <t>TC003_09</t>
+  </si>
+  <si>
+    <t>TC003_10</t>
+  </si>
+  <si>
+    <t>TC003_11</t>
+  </si>
+  <si>
+    <t>TC003_12</t>
+  </si>
+  <si>
+    <t>TC003_13</t>
+  </si>
+  <si>
+    <t>TC003_14</t>
+  </si>
+  <si>
+    <t>Verify quantity of the product</t>
+  </si>
+  <si>
+    <t>Verify price of the product</t>
+  </si>
+  <si>
+    <t>storeValue</t>
+  </si>
+  <si>
+    <t>mouseHover</t>
+  </si>
+  <si>
+    <t>verifyStoredText</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
     <t>PASS</t>
-  </si>
-  <si>
-    <t>firefox</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>TC003</t>
-  </si>
-  <si>
-    <t>Add a product to cart</t>
-  </si>
-  <si>
-    <t>TC003_01</t>
-  </si>
-  <si>
-    <t>Click on Product Category</t>
-  </si>
-  <si>
-    <t>Click on iPhones</t>
-  </si>
-  <si>
-    <t>Verify and store product price</t>
-  </si>
-  <si>
-    <t>Add product to Cart</t>
-  </si>
-  <si>
-    <t>Navigate to Cart</t>
-  </si>
-  <si>
-    <t>TC004</t>
-  </si>
-  <si>
-    <t>TC003_02</t>
-  </si>
-  <si>
-    <t>TC003_03</t>
-  </si>
-  <si>
-    <t>TC003_04</t>
-  </si>
-  <si>
-    <t>TC003_05</t>
-  </si>
-  <si>
-    <t>TC003_06</t>
-  </si>
-  <si>
-    <t>TC003_07</t>
-  </si>
-  <si>
-    <t>TC003_08</t>
-  </si>
-  <si>
-    <t>TC003_09</t>
-  </si>
-  <si>
-    <t>TC003_10</t>
-  </si>
-  <si>
-    <t>TC003_11</t>
-  </si>
-  <si>
-    <t>TC003_12</t>
-  </si>
-  <si>
-    <t>TC003_13</t>
-  </si>
-  <si>
-    <t>TC003_14</t>
-  </si>
-  <si>
-    <t>Verify quantity of the product</t>
-  </si>
-  <si>
-    <t>Verify price of the product</t>
-  </si>
-  <si>
-    <t>storeValue</t>
   </si>
 </sst>
 </file>
@@ -727,7 +733,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -870,6 +876,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -919,7 +936,7 @@
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -930,6 +947,14 @@
     <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="20" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" hidden="1"/>
@@ -1290,16 +1315,16 @@
   <sheetPr codeName="Blad2"/>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="56.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="56.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1324,7 +1349,10 @@
         <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>54</v>
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1335,18 +1363,21 @@
         <v>37</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>54</v>
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1371,18 +1402,18 @@
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="37" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="6" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="4" max="6" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="15" width="24.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1404,7 +1435,7 @@
       <c r="F1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="11" t="s">
         <v>64</v>
       </c>
       <c r="H1" s="9" t="s">
@@ -1426,11 +1457,11 @@
       <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="12" t="s">
         <v>82</v>
       </c>
       <c r="H2" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1448,9 +1479,9 @@
       <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="4"/>
+      <c r="G3" s="12"/>
       <c r="H3" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1472,9 +1503,9 @@
       <c r="F4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="4"/>
+      <c r="G4" s="12"/>
       <c r="H4" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1496,11 +1527,11 @@
       <c r="F5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="12" t="s">
         <v>33</v>
       </c>
       <c r="H5" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1522,11 +1553,11 @@
       <c r="F6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="12" t="s">
         <v>34</v>
       </c>
       <c r="H6" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1548,9 +1579,9 @@
       <c r="F7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="4"/>
+      <c r="G7" s="12"/>
       <c r="H7" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1568,9 +1599,9 @@
       <c r="F8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="4"/>
+      <c r="G8" s="12"/>
       <c r="H8" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1592,9 +1623,9 @@
       <c r="F9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="4"/>
+      <c r="G9" s="12"/>
       <c r="H9" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1612,9 +1643,9 @@
       <c r="F10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="4"/>
+      <c r="G10" s="12"/>
       <c r="H10" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1632,11 +1663,11 @@
       <c r="F11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>84</v>
+      <c r="G11" s="13" t="s">
+        <v>83</v>
       </c>
       <c r="H11" t="s">
-        <v>85</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1654,7 +1685,10 @@
       <c r="F12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="13"/>
+      <c r="H12" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -1675,7 +1709,10 @@
       <c r="F13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="3"/>
+      <c r="G13" s="13"/>
+      <c r="H13" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -1696,7 +1733,7 @@
       <c r="F14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="13" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1719,7 +1756,7 @@
       <c r="F15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="13" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1742,7 +1779,7 @@
       <c r="F16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G16" s="3"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
@@ -1759,7 +1796,7 @@
       <c r="F17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="3"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -1780,7 +1817,7 @@
       <c r="F18" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="13" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1799,14 +1836,14 @@
       <c r="F19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="3"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>88</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>16</v>
@@ -1816,16 +1853,16 @@
       <c r="F20" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="12" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>17</v>
@@ -1835,14 +1872,14 @@
       <c r="F21" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G21" s="4"/>
+      <c r="G21" s="12"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>18</v>
@@ -1856,14 +1893,14 @@
       <c r="F22" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G22" s="4"/>
+      <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>19</v>
@@ -1877,16 +1914,16 @@
       <c r="F23" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>20</v>
@@ -1900,16 +1937,16 @@
       <c r="F24" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G24" s="12" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>21</v>
@@ -1923,14 +1960,14 @@
       <c r="F25" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G25" s="4"/>
+      <c r="G25" s="12"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>22</v>
@@ -1940,17 +1977,17 @@
       <c r="F26" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G26" s="4"/>
+      <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>68</v>
@@ -1959,19 +1996,19 @@
         <v>72</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G27" s="4"/>
+        <v>109</v>
+      </c>
+      <c r="G27" s="12"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>68</v>
@@ -1982,17 +2019,17 @@
       <c r="F28" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G28" s="4"/>
+      <c r="G28" s="12"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>68</v>
@@ -2001,19 +2038,19 @@
         <v>75</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G29" s="4"/>
+        <v>108</v>
+      </c>
+      <c r="G29" s="12"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>68</v>
@@ -2024,17 +2061,17 @@
       <c r="F30" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G30" s="4"/>
+      <c r="G30" s="12"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>68</v>
@@ -2045,17 +2082,17 @@
       <c r="F31" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G31" s="4"/>
+      <c r="G31" s="12"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>69</v>
@@ -2066,17 +2103,19 @@
       <c r="F32" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G32" s="4"/>
+      <c r="G32" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B33" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>109</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>69</v>
@@ -2085,9 +2124,9 @@
         <v>81</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G33" s="4"/>
+        <v>110</v>
+      </c>
+      <c r="G33" s="12"/>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -2108,21 +2147,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="26" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2293,6 +2332,16 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F11" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F12" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Made changes to Extent Report
</commit_message>
<xml_diff>
--- a/bin/dataEngine/DataEngine.xlsx
+++ b/bin/dataEngine/DataEngine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="11295" windowHeight="8130" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="11295" windowHeight="8130"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="112">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -275,9 +275,6 @@
     <t>chrome</t>
   </si>
   <si>
-    <t>firefox</t>
-  </si>
-  <si>
     <t>TC003</t>
   </si>
   <si>
@@ -290,79 +287,79 @@
     <t>Click on Product Category</t>
   </si>
   <si>
+    <t>Verify and store product price</t>
+  </si>
+  <si>
+    <t>Add product to Cart</t>
+  </si>
+  <si>
+    <t>Navigate to Cart</t>
+  </si>
+  <si>
+    <t>TC004</t>
+  </si>
+  <si>
+    <t>TC003_02</t>
+  </si>
+  <si>
+    <t>TC003_03</t>
+  </si>
+  <si>
+    <t>TC003_04</t>
+  </si>
+  <si>
+    <t>TC003_05</t>
+  </si>
+  <si>
+    <t>TC003_06</t>
+  </si>
+  <si>
+    <t>TC003_07</t>
+  </si>
+  <si>
+    <t>TC003_08</t>
+  </si>
+  <si>
+    <t>TC003_09</t>
+  </si>
+  <si>
+    <t>TC003_10</t>
+  </si>
+  <si>
+    <t>TC003_11</t>
+  </si>
+  <si>
+    <t>TC003_12</t>
+  </si>
+  <si>
+    <t>TC003_13</t>
+  </si>
+  <si>
+    <t>TC003_14</t>
+  </si>
+  <si>
+    <t>Verify quantity of the product</t>
+  </si>
+  <si>
+    <t>Verify price of the product</t>
+  </si>
+  <si>
+    <t>storeValue</t>
+  </si>
+  <si>
+    <t>mouseHover</t>
+  </si>
+  <si>
+    <t>verifyStoredText</t>
+  </si>
+  <si>
     <t>Click on iPhones</t>
   </si>
   <si>
-    <t>Verify and store product price</t>
-  </si>
-  <si>
-    <t>Add product to Cart</t>
-  </si>
-  <si>
-    <t>Navigate to Cart</t>
-  </si>
-  <si>
-    <t>TC004</t>
-  </si>
-  <si>
-    <t>TC003_02</t>
-  </si>
-  <si>
-    <t>TC003_03</t>
-  </si>
-  <si>
-    <t>TC003_04</t>
-  </si>
-  <si>
-    <t>TC003_05</t>
-  </si>
-  <si>
-    <t>TC003_06</t>
-  </si>
-  <si>
-    <t>TC003_07</t>
-  </si>
-  <si>
-    <t>TC003_08</t>
-  </si>
-  <si>
-    <t>TC003_09</t>
-  </si>
-  <si>
-    <t>TC003_10</t>
-  </si>
-  <si>
-    <t>TC003_11</t>
-  </si>
-  <si>
-    <t>TC003_12</t>
-  </si>
-  <si>
-    <t>TC003_13</t>
-  </si>
-  <si>
-    <t>TC003_14</t>
-  </si>
-  <si>
-    <t>Verify quantity of the product</t>
-  </si>
-  <si>
-    <t>Verify price of the product</t>
-  </si>
-  <si>
-    <t>storeValue</t>
-  </si>
-  <si>
-    <t>mouseHover</t>
-  </si>
-  <si>
-    <t>verifyStoredText</t>
+    <t>PASS</t>
   </si>
   <si>
     <t>FAIL</t>
-  </si>
-  <si>
-    <t>PASS</t>
   </si>
 </sst>
 </file>
@@ -1315,8 +1312,8 @@
   <sheetPr codeName="Blad2"/>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1352,7 +1349,7 @@
         <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1363,21 +1360,21 @@
         <v>37</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" t="s">
-        <v>111</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>54</v>
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1402,8 +1399,8 @@
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,7 +1458,7 @@
         <v>82</v>
       </c>
       <c r="H2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1481,7 +1478,7 @@
       </c>
       <c r="G3" s="12"/>
       <c r="H3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1505,7 +1502,7 @@
       </c>
       <c r="G4" s="12"/>
       <c r="H4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1531,7 +1528,7 @@
         <v>33</v>
       </c>
       <c r="H5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1557,7 +1554,7 @@
         <v>34</v>
       </c>
       <c r="H6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1581,7 +1578,7 @@
       </c>
       <c r="G7" s="12"/>
       <c r="H7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1601,7 +1598,7 @@
       </c>
       <c r="G8" s="12"/>
       <c r="H8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1625,7 +1622,7 @@
       </c>
       <c r="G9" s="12"/>
       <c r="H9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1645,7 +1642,7 @@
       </c>
       <c r="G10" s="12"/>
       <c r="H10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1664,10 +1661,7 @@
         <v>4</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="H11" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1686,9 +1680,6 @@
         <v>5</v>
       </c>
       <c r="G12" s="13"/>
-      <c r="H12" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -1710,9 +1701,6 @@
         <v>31</v>
       </c>
       <c r="G13" s="13"/>
-      <c r="H13" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -1840,10 +1828,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>16</v>
@@ -1856,13 +1844,16 @@
       <c r="G20" s="12" t="s">
         <v>82</v>
       </c>
+      <c r="H20" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>17</v>
@@ -1873,13 +1864,16 @@
         <v>5</v>
       </c>
       <c r="G21" s="12"/>
+      <c r="H21" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>18</v>
@@ -1894,13 +1888,16 @@
         <v>31</v>
       </c>
       <c r="G22" s="12"/>
+      <c r="H22" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>19</v>
@@ -1917,13 +1914,16 @@
       <c r="G23" s="12" t="s">
         <v>33</v>
       </c>
+      <c r="H23" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>20</v>
@@ -1940,13 +1940,16 @@
       <c r="G24" s="12" t="s">
         <v>34</v>
       </c>
+      <c r="H24" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>21</v>
@@ -1961,13 +1964,16 @@
         <v>31</v>
       </c>
       <c r="G25" s="12"/>
+      <c r="H25" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>22</v>
@@ -1978,16 +1984,19 @@
         <v>6</v>
       </c>
       <c r="G26" s="12"/>
+      <c r="H26" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>68</v>
@@ -1996,19 +2005,22 @@
         <v>72</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G27" s="12"/>
+      <c r="H27" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>68</v>
@@ -2020,16 +2032,19 @@
         <v>31</v>
       </c>
       <c r="G28" s="12"/>
+      <c r="H28" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>68</v>
@@ -2038,19 +2053,19 @@
         <v>75</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G29" s="12"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>68</v>
@@ -2065,13 +2080,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>68</v>
@@ -2086,13 +2101,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>69</v>
@@ -2109,13 +2124,13 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B33" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>69</v>
@@ -2124,7 +2139,7 @@
         <v>81</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G33" s="12"/>
     </row>
@@ -2332,17 +2347,17 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F11" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F12" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes made on 27 Apr 16
</commit_message>
<xml_diff>
--- a/bin/dataEngine/DataEngine.xlsx
+++ b/bin/dataEngine/DataEngine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="11295" windowHeight="8130"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="11295" windowHeight="8130" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="108">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -335,9 +335,6 @@
     <t>TC003_13</t>
   </si>
   <si>
-    <t>TC003_14</t>
-  </si>
-  <si>
     <t>Verify quantity of the product</t>
   </si>
   <si>
@@ -351,15 +348,6 @@
   </si>
   <si>
     <t>verifyStoredText</t>
-  </si>
-  <si>
-    <t>Click on iPhones</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -1312,16 +1300,16 @@
   <sheetPr codeName="Blad2"/>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="56.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="56.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1346,10 +1334,7 @@
         <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>110</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1372,9 +1357,6 @@
       </c>
       <c r="C4" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="D4" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1397,20 +1379,20 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Blad1"/>
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17:H31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="37.0" collapsed="true"/>
-    <col min="4" max="6" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="15" width="24.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="6" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="24.140625" style="15" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1457,9 +1439,6 @@
       <c r="G2" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="H2" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1477,9 +1456,6 @@
         <v>5</v>
       </c>
       <c r="G3" s="12"/>
-      <c r="H3" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1501,9 +1477,6 @@
         <v>31</v>
       </c>
       <c r="G4" s="12"/>
-      <c r="H4" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -1527,9 +1500,6 @@
       <c r="G5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="H5" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -1553,9 +1523,6 @@
       <c r="G6" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="H6" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -1577,9 +1544,6 @@
         <v>31</v>
       </c>
       <c r="G7" s="12"/>
-      <c r="H7" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1597,9 +1561,6 @@
         <v>6</v>
       </c>
       <c r="G8" s="12"/>
-      <c r="H8" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -1621,9 +1582,6 @@
         <v>31</v>
       </c>
       <c r="G9" s="12"/>
-      <c r="H9" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -1641,9 +1599,6 @@
         <v>7</v>
       </c>
       <c r="G10" s="12"/>
-      <c r="H10" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -1844,9 +1799,6 @@
       <c r="G20" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="H20" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
@@ -1864,9 +1816,6 @@
         <v>5</v>
       </c>
       <c r="G21" s="12"/>
-      <c r="H21" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
@@ -1888,9 +1837,6 @@
         <v>31</v>
       </c>
       <c r="G22" s="12"/>
-      <c r="H22" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
@@ -1914,9 +1860,6 @@
       <c r="G23" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="H23" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
@@ -1940,9 +1883,6 @@
       <c r="G24" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="H24" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
@@ -1964,9 +1904,6 @@
         <v>31</v>
       </c>
       <c r="G25" s="12"/>
-      <c r="H25" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
@@ -1984,9 +1921,6 @@
         <v>6</v>
       </c>
       <c r="G26" s="12"/>
-      <c r="H26" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
@@ -2005,11 +1939,10 @@
         <v>72</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="G27" s="12"/>
-      <c r="H27" t="s">
-        <v>110</v>
+        <v>106</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -2020,21 +1953,18 @@
         <v>98</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>31</v>
+        <v>105</v>
       </c>
       <c r="G28" s="12"/>
-      <c r="H28" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
@@ -2044,16 +1974,16 @@
         <v>99</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>106</v>
+        <v>31</v>
       </c>
       <c r="G29" s="12"/>
     </row>
@@ -2065,13 +1995,13 @@
         <v>100</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>31</v>
@@ -2086,22 +2016,24 @@
         <v>101</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G31" s="12"/>
+        <v>50</v>
+      </c>
+      <c r="G31" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>102</v>
@@ -2113,45 +2045,22 @@
         <v>69</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G32" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="G33" s="12"/>
+        <v>107</v>
+      </c>
+      <c r="G32" s="12"/>
     </row>
   </sheetData>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D19">
       <formula1>PageName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E32">
       <formula1>INDIRECT(D2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F32">
       <formula1>ActionKeywords</formula1>
     </dataValidation>
   </dataValidations>
@@ -2170,13 +2079,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="27.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2347,17 +2256,17 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F11" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F12" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit on 29 Apr 16
</commit_message>
<xml_diff>
--- a/bin/dataEngine/DataEngine.xlsx
+++ b/bin/dataEngine/DataEngine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="11295" windowHeight="8130" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="11295" windowHeight="8130"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="109">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -348,6 +348,9 @@
   </si>
   <si>
     <t>verifyStoredText</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
@@ -1300,16 +1303,16 @@
   <sheetPr codeName="Blad2"/>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="56.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="56.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1381,18 +1384,18 @@
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="37" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="6" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.140625" style="15" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="4" max="6" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="15" width="24.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1799,6 +1802,9 @@
       <c r="G20" s="12" t="s">
         <v>82</v>
       </c>
+      <c r="H20" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
@@ -1816,6 +1822,9 @@
         <v>5</v>
       </c>
       <c r="G21" s="12"/>
+      <c r="H21" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
@@ -1837,6 +1846,9 @@
         <v>31</v>
       </c>
       <c r="G22" s="12"/>
+      <c r="H22" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
@@ -1860,6 +1872,9 @@
       <c r="G23" s="12" t="s">
         <v>33</v>
       </c>
+      <c r="H23" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
@@ -1883,6 +1898,9 @@
       <c r="G24" s="12" t="s">
         <v>34</v>
       </c>
+      <c r="H24" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
@@ -1904,6 +1922,9 @@
         <v>31</v>
       </c>
       <c r="G25" s="12"/>
+      <c r="H25" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
@@ -1921,6 +1942,9 @@
         <v>6</v>
       </c>
       <c r="G26" s="12"/>
+      <c r="H26" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
@@ -1944,6 +1968,9 @@
       <c r="G27" s="12" t="s">
         <v>73</v>
       </c>
+      <c r="H27" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
@@ -1965,6 +1992,9 @@
         <v>105</v>
       </c>
       <c r="G28" s="12"/>
+      <c r="H28" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
@@ -1986,6 +2016,9 @@
         <v>31</v>
       </c>
       <c r="G29" s="12"/>
+      <c r="H29" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
@@ -2007,6 +2040,9 @@
         <v>31</v>
       </c>
       <c r="G30" s="12"/>
+      <c r="H30" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
@@ -2079,13 +2115,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="26" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
2nd Commit on 29 Apr 16
</commit_message>
<xml_diff>
--- a/bin/dataEngine/DataEngine.xlsx
+++ b/bin/dataEngine/DataEngine.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="112">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -176,9 +176,6 @@
     <t>Verify error message</t>
   </si>
   <si>
-    <t>verify</t>
-  </si>
-  <si>
     <t>Invalid login credentials</t>
   </si>
   <si>
@@ -296,9 +293,6 @@
     <t>Navigate to Cart</t>
   </si>
   <si>
-    <t>TC004</t>
-  </si>
-  <si>
     <t>TC003_02</t>
   </si>
   <si>
@@ -350,7 +344,22 @@
     <t>verifyStoredText</t>
   </si>
   <si>
+    <t>verifyValue</t>
+  </si>
+  <si>
+    <t>verifyText</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>TC003_14</t>
+  </si>
+  <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -868,11 +877,13 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -924,7 +935,7 @@
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -935,14 +946,17 @@
     <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="20" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="34" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" hidden="1"/>
@@ -1323,10 +1337,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1337,7 +1351,7 @@
         <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1348,18 +1362,21 @@
         <v>37</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1382,10 +1399,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Blad1"/>
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17:H33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19:H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1394,34 +1411,34 @@
     <col min="2" max="2" customWidth="true" width="13.85546875" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="37.0" collapsed="true"/>
     <col min="4" max="6" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="15" width="24.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="13" width="24.140625" collapsed="true"/>
     <col min="8" max="8" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>67</v>
-      </c>
       <c r="D1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>63</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="11" t="s">
-        <v>64</v>
+      <c r="G1" s="10" t="s">
+        <v>63</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1439,8 +1456,8 @@
       <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>82</v>
+      <c r="G2" s="11" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1458,7 +1475,7 @@
       <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="12"/>
+      <c r="G3" s="11"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1471,7 +1488,7 @@
         <v>18</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>26</v>
@@ -1479,7 +1496,7 @@
       <c r="F4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="12"/>
+      <c r="G4" s="11"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -1492,7 +1509,7 @@
         <v>19</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>30</v>
@@ -1500,7 +1517,7 @@
       <c r="F5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1515,7 +1532,7 @@
         <v>20</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>27</v>
@@ -1523,7 +1540,7 @@
       <c r="F6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="11" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1538,7 +1555,7 @@
         <v>21</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>28</v>
@@ -1546,7 +1563,7 @@
       <c r="F7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="12"/>
+      <c r="G7" s="11"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1563,7 +1580,7 @@
       <c r="F8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="12"/>
+      <c r="G8" s="11"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -1576,7 +1593,7 @@
         <v>23</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>29</v>
@@ -1584,7 +1601,7 @@
       <c r="F9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="12"/>
+      <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -1601,7 +1618,7 @@
       <c r="F10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="12"/>
+      <c r="G10" s="11"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -1618,8 +1635,8 @@
       <c r="F11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="13" t="s">
-        <v>82</v>
+      <c r="G11" s="12" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1637,7 +1654,7 @@
       <c r="F12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="13"/>
+      <c r="G12" s="12"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -1650,7 +1667,7 @@
         <v>18</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>26</v>
@@ -1658,7 +1675,7 @@
       <c r="F13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="13"/>
+      <c r="G13" s="12"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -1671,7 +1688,7 @@
         <v>19</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>30</v>
@@ -1679,7 +1696,7 @@
       <c r="F14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="12" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1694,7 +1711,7 @@
         <v>20</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>27</v>
@@ -1702,7 +1719,7 @@
       <c r="F15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="13" t="s">
+      <c r="G15" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1717,7 +1734,7 @@
         <v>21</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>28</v>
@@ -1725,7 +1742,7 @@
       <c r="F16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G16" s="13"/>
+      <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
@@ -1742,7 +1759,7 @@
       <c r="F17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="13"/>
+      <c r="G17" s="12"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -1755,16 +1772,16 @@
         <v>49</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F18" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" s="12" t="s">
         <v>50</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1782,14 +1799,14 @@
       <c r="F19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="13"/>
+      <c r="G19" s="12"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>16</v>
@@ -1799,19 +1816,19 @@
       <c r="F20" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="12" t="s">
-        <v>82</v>
+      <c r="G20" s="11" t="s">
+        <v>81</v>
       </c>
       <c r="H20" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>17</v>
@@ -1821,23 +1838,23 @@
       <c r="F21" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G21" s="12"/>
+      <c r="G21" s="11"/>
       <c r="H21" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>26</v>
@@ -1845,23 +1862,23 @@
       <c r="F22" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G22" s="12"/>
+      <c r="G22" s="11"/>
       <c r="H22" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>30</v>
@@ -1869,25 +1886,25 @@
       <c r="F23" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G23" s="12" t="s">
+      <c r="G23" s="11" t="s">
         <v>33</v>
       </c>
       <c r="H23" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>27</v>
@@ -1895,25 +1912,25 @@
       <c r="F24" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G24" s="12" t="s">
+      <c r="G24" s="11" t="s">
         <v>34</v>
       </c>
       <c r="H24" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>28</v>
@@ -1921,17 +1938,17 @@
       <c r="F25" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G25" s="12"/>
+      <c r="G25" s="11"/>
       <c r="H25" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>22</v>
@@ -1941,162 +1958,188 @@
       <c r="F26" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G26" s="12"/>
+      <c r="G26" s="11"/>
       <c r="H26" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E27" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G27" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>73</v>
-      </c>
       <c r="H27" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="G28" s="12"/>
+        <v>103</v>
+      </c>
+      <c r="G28" s="11"/>
       <c r="H28" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G29" s="12"/>
+      <c r="G29" s="11"/>
       <c r="H29" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G30" s="12"/>
+      <c r="G30" s="11"/>
       <c r="H30" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B31" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>103</v>
-      </c>
       <c r="D31" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G31" s="14">
-        <v>1</v>
+        <v>106</v>
+      </c>
+      <c r="G31" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="H31" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>104</v>
-      </c>
       <c r="D32" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="G32" s="12"/>
+        <v>105</v>
+      </c>
+      <c r="G32" s="11"/>
+      <c r="H32" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G33" s="11"/>
+      <c r="H33" t="s">
+        <v>110</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D19 D33">
       <formula1>PageName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E33">
       <formula1>INDIRECT(D2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F33">
       <formula1>ActionKeywords</formula1>
     </dataValidation>
   </dataValidations>
@@ -2107,10 +2150,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2126,30 +2169,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="D1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>71</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>26</v>
@@ -2158,21 +2201,21 @@
         <v>30</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>76</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="16" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>29</v>
@@ -2181,129 +2224,164 @@
         <v>27</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>77</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>54</v>
+      <c r="G3" s="16" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="16"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>80</v>
+        <v>74</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>79</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="16"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>80</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="16"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="15"/>
       <c r="F7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="2"/>
+      <c r="G7" s="16"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="15"/>
       <c r="F8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="2"/>
+      <c r="G8" s="16"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="E9" s="15"/>
       <c r="F9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="2"/>
+      <c r="G9" s="16"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="15"/>
       <c r="F10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" s="2"/>
+        <v>106</v>
+      </c>
+      <c r="G10" s="16"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F11" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F12" s="17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F13" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F12" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F13" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F14" s="2" t="s">
         <v>107</v>
       </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
3rd Commit on 29 Apr 16
</commit_message>
<xml_diff>
--- a/bin/dataEngine/DataEngine.xlsx
+++ b/bin/dataEngine/DataEngine.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="112">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1318,7 +1318,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,7 +1351,10 @@
         <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>53</v>
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1362,7 +1365,10 @@
         <v>37</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>53</v>
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1402,7 +1408,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19:H34"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,6 +1465,9 @@
       <c r="G2" s="11" t="s">
         <v>81</v>
       </c>
+      <c r="H2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1476,6 +1485,9 @@
         <v>5</v>
       </c>
       <c r="G3" s="11"/>
+      <c r="H3" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1497,6 +1509,9 @@
         <v>31</v>
       </c>
       <c r="G4" s="11"/>
+      <c r="H4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -1520,6 +1535,9 @@
       <c r="G5" s="11" t="s">
         <v>33</v>
       </c>
+      <c r="H5" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -1543,6 +1561,9 @@
       <c r="G6" s="11" t="s">
         <v>34</v>
       </c>
+      <c r="H6" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -1564,6 +1585,9 @@
         <v>31</v>
       </c>
       <c r="G7" s="11"/>
+      <c r="H7" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1581,6 +1605,9 @@
         <v>6</v>
       </c>
       <c r="G8" s="11"/>
+      <c r="H8" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -1602,6 +1629,9 @@
         <v>31</v>
       </c>
       <c r="G9" s="11"/>
+      <c r="H9" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -1619,6 +1649,9 @@
         <v>7</v>
       </c>
       <c r="G10" s="11"/>
+      <c r="H10" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -1638,6 +1671,9 @@
       <c r="G11" s="12" t="s">
         <v>81</v>
       </c>
+      <c r="H11" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1655,6 +1691,9 @@
         <v>5</v>
       </c>
       <c r="G12" s="12"/>
+      <c r="H12" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -1676,6 +1715,9 @@
         <v>31</v>
       </c>
       <c r="G13" s="12"/>
+      <c r="H13" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -1699,6 +1741,9 @@
       <c r="G14" s="12" t="s">
         <v>48</v>
       </c>
+      <c r="H14" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -1722,6 +1767,9 @@
       <c r="G15" s="12" t="s">
         <v>34</v>
       </c>
+      <c r="H15" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -1743,6 +1791,9 @@
         <v>31</v>
       </c>
       <c r="G16" s="12"/>
+      <c r="H16" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
@@ -1760,6 +1811,9 @@
         <v>6</v>
       </c>
       <c r="G17" s="12"/>
+      <c r="H17" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -1782,6 +1836,9 @@
       </c>
       <c r="G18" s="12" t="s">
         <v>50</v>
+      </c>
+      <c r="H18" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1800,6 +1857,9 @@
         <v>7</v>
       </c>
       <c r="G19" s="12"/>
+      <c r="H19" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">

</xml_diff>

<commit_message>
1st Commit on 3rd May
</commit_message>
<xml_diff>
--- a/bin/dataEngine/DataEngine.xlsx
+++ b/bin/dataEngine/DataEngine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="11295" windowHeight="8130"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="11295" windowHeight="8130" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="112">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -354,6 +354,12 @@
   </si>
   <si>
     <t>TC003_14</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -1311,16 +1317,16 @@
   <sheetPr codeName="Blad2"/>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="56.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="56.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1347,6 +1353,9 @@
       <c r="C2" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="D2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1358,6 +1367,9 @@
       <c r="C3" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="D3" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1368,6 +1380,9 @@
       </c>
       <c r="C4" s="2" t="s">
         <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1392,18 +1407,18 @@
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="37" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="6" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.140625" style="13" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="4" max="6" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="13" width="24.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1450,6 +1465,9 @@
       <c r="G2" s="11" t="s">
         <v>81</v>
       </c>
+      <c r="H2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1467,6 +1485,9 @@
         <v>5</v>
       </c>
       <c r="G3" s="11"/>
+      <c r="H3" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1488,6 +1509,9 @@
         <v>31</v>
       </c>
       <c r="G4" s="11"/>
+      <c r="H4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -1511,6 +1535,9 @@
       <c r="G5" s="11" t="s">
         <v>33</v>
       </c>
+      <c r="H5" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -1534,6 +1561,9 @@
       <c r="G6" s="11" t="s">
         <v>34</v>
       </c>
+      <c r="H6" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -1555,6 +1585,9 @@
         <v>31</v>
       </c>
       <c r="G7" s="11"/>
+      <c r="H7" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1572,6 +1605,9 @@
         <v>6</v>
       </c>
       <c r="G8" s="11"/>
+      <c r="H8" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -1593,6 +1629,9 @@
         <v>31</v>
       </c>
       <c r="G9" s="11"/>
+      <c r="H9" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -1610,6 +1649,9 @@
         <v>7</v>
       </c>
       <c r="G10" s="11"/>
+      <c r="H10" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -1629,6 +1671,9 @@
       <c r="G11" s="12" t="s">
         <v>81</v>
       </c>
+      <c r="H11" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1646,6 +1691,9 @@
         <v>5</v>
       </c>
       <c r="G12" s="12"/>
+      <c r="H12" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -1667,6 +1715,9 @@
         <v>31</v>
       </c>
       <c r="G13" s="12"/>
+      <c r="H13" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -1690,6 +1741,9 @@
       <c r="G14" s="12" t="s">
         <v>48</v>
       </c>
+      <c r="H14" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -1713,6 +1767,9 @@
       <c r="G15" s="12" t="s">
         <v>34</v>
       </c>
+      <c r="H15" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -1734,6 +1791,9 @@
         <v>31</v>
       </c>
       <c r="G16" s="12"/>
+      <c r="H16" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
@@ -1751,6 +1811,9 @@
         <v>6</v>
       </c>
       <c r="G17" s="12"/>
+      <c r="H17" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -1773,6 +1836,9 @@
       </c>
       <c r="G18" s="12" t="s">
         <v>50</v>
+      </c>
+      <c r="H18" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1791,6 +1857,9 @@
         <v>7</v>
       </c>
       <c r="G19" s="12"/>
+      <c r="H19" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
@@ -1810,6 +1879,9 @@
       <c r="G20" s="11" t="s">
         <v>81</v>
       </c>
+      <c r="H20" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
@@ -1827,6 +1899,9 @@
         <v>5</v>
       </c>
       <c r="G21" s="11"/>
+      <c r="H21" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
@@ -1848,6 +1923,9 @@
         <v>31</v>
       </c>
       <c r="G22" s="11"/>
+      <c r="H22" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
@@ -1871,6 +1949,9 @@
       <c r="G23" s="11" t="s">
         <v>33</v>
       </c>
+      <c r="H23" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
@@ -1894,6 +1975,9 @@
       <c r="G24" s="11" t="s">
         <v>34</v>
       </c>
+      <c r="H24" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
@@ -1915,6 +1999,9 @@
         <v>31</v>
       </c>
       <c r="G25" s="11"/>
+      <c r="H25" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
@@ -1932,6 +2019,9 @@
         <v>6</v>
       </c>
       <c r="G26" s="11"/>
+      <c r="H26" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
@@ -1955,6 +2045,9 @@
       <c r="G27" s="11" t="s">
         <v>72</v>
       </c>
+      <c r="H27" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
@@ -1976,6 +2069,9 @@
         <v>103</v>
       </c>
       <c r="G28" s="11"/>
+      <c r="H28" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
@@ -1997,6 +2093,9 @@
         <v>31</v>
       </c>
       <c r="G29" s="11"/>
+      <c r="H29" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
@@ -2018,6 +2117,9 @@
         <v>31</v>
       </c>
       <c r="G30" s="11"/>
+      <c r="H30" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
@@ -2041,6 +2143,9 @@
       <c r="G31" s="18" t="s">
         <v>108</v>
       </c>
+      <c r="H31" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
@@ -2062,6 +2167,9 @@
         <v>105</v>
       </c>
       <c r="G32" s="11"/>
+      <c r="H32" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
@@ -2079,6 +2187,9 @@
         <v>7</v>
       </c>
       <c r="G33" s="11"/>
+      <c r="H33" t="s">
+        <v>110</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -2107,13 +2218,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="26" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added WinForm to execute Driver Script
</commit_message>
<xml_diff>
--- a/bin/dataEngine/DataEngine.xlsx
+++ b/bin/dataEngine/DataEngine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="11295" windowHeight="8130" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="11295" windowHeight="8130"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="110">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -354,12 +354,6 @@
   </si>
   <si>
     <t>TC003_14</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -1317,16 +1311,16 @@
   <sheetPr codeName="Blad2"/>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="56.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="56.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1353,9 +1347,6 @@
       <c r="C2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D2" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1367,9 +1358,6 @@
       <c r="C3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D3" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1380,9 +1368,6 @@
       </c>
       <c r="C4" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="D4" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1407,18 +1392,18 @@
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="37.0" collapsed="true"/>
-    <col min="4" max="6" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="13" width="24.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="6" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="24.140625" style="13" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1465,9 +1450,6 @@
       <c r="G2" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="H2" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1485,9 +1467,6 @@
         <v>5</v>
       </c>
       <c r="G3" s="11"/>
-      <c r="H3" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1509,9 +1488,6 @@
         <v>31</v>
       </c>
       <c r="G4" s="11"/>
-      <c r="H4" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -1535,9 +1511,6 @@
       <c r="G5" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="H5" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -1561,9 +1534,6 @@
       <c r="G6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H6" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -1585,9 +1555,6 @@
         <v>31</v>
       </c>
       <c r="G7" s="11"/>
-      <c r="H7" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1605,9 +1572,6 @@
         <v>6</v>
       </c>
       <c r="G8" s="11"/>
-      <c r="H8" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -1629,9 +1593,6 @@
         <v>31</v>
       </c>
       <c r="G9" s="11"/>
-      <c r="H9" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -1649,9 +1610,6 @@
         <v>7</v>
       </c>
       <c r="G10" s="11"/>
-      <c r="H10" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -1671,9 +1629,6 @@
       <c r="G11" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="H11" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1691,9 +1646,6 @@
         <v>5</v>
       </c>
       <c r="G12" s="12"/>
-      <c r="H12" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -1715,9 +1667,6 @@
         <v>31</v>
       </c>
       <c r="G13" s="12"/>
-      <c r="H13" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -1741,9 +1690,6 @@
       <c r="G14" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="H14" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -1767,9 +1713,6 @@
       <c r="G15" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="H15" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -1791,9 +1734,6 @@
         <v>31</v>
       </c>
       <c r="G16" s="12"/>
-      <c r="H16" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
@@ -1811,9 +1751,6 @@
         <v>6</v>
       </c>
       <c r="G17" s="12"/>
-      <c r="H17" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -1836,9 +1773,6 @@
       </c>
       <c r="G18" s="12" t="s">
         <v>50</v>
-      </c>
-      <c r="H18" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1857,9 +1791,6 @@
         <v>7</v>
       </c>
       <c r="G19" s="12"/>
-      <c r="H19" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
@@ -1879,9 +1810,6 @@
       <c r="G20" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="H20" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
@@ -1899,9 +1827,6 @@
         <v>5</v>
       </c>
       <c r="G21" s="11"/>
-      <c r="H21" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
@@ -1923,9 +1848,6 @@
         <v>31</v>
       </c>
       <c r="G22" s="11"/>
-      <c r="H22" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
@@ -1949,9 +1871,6 @@
       <c r="G23" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="H23" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
@@ -1975,9 +1894,6 @@
       <c r="G24" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H24" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
@@ -1999,9 +1915,6 @@
         <v>31</v>
       </c>
       <c r="G25" s="11"/>
-      <c r="H25" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
@@ -2019,9 +1932,6 @@
         <v>6</v>
       </c>
       <c r="G26" s="11"/>
-      <c r="H26" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
@@ -2045,9 +1955,6 @@
       <c r="G27" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="H27" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
@@ -2069,9 +1976,6 @@
         <v>103</v>
       </c>
       <c r="G28" s="11"/>
-      <c r="H28" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
@@ -2093,9 +1997,6 @@
         <v>31</v>
       </c>
       <c r="G29" s="11"/>
-      <c r="H29" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
@@ -2117,9 +2018,6 @@
         <v>31</v>
       </c>
       <c r="G30" s="11"/>
-      <c r="H30" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
@@ -2143,9 +2041,6 @@
       <c r="G31" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="H31" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
@@ -2167,9 +2062,6 @@
         <v>105</v>
       </c>
       <c r="G32" s="11"/>
-      <c r="H32" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
@@ -2187,9 +2079,6 @@
         <v>7</v>
       </c>
       <c r="G33" s="11"/>
-      <c r="H33" t="s">
-        <v>110</v>
-      </c>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -2218,13 +2107,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="27.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
1st Commit on 4th May 16
</commit_message>
<xml_diff>
--- a/bin/dataEngine/DataEngine.xlsx
+++ b/bin/dataEngine/DataEngine.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="112">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -354,6 +354,12 @@
   </si>
   <si>
     <t>TC003_14</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -1317,10 +1323,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="56.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="56.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1347,6 +1353,9 @@
       <c r="C2" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="D2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1358,6 +1367,9 @@
       <c r="C3" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="D3" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1368,6 +1380,9 @@
       </c>
       <c r="C4" s="2" t="s">
         <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1398,12 +1413,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="37" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="6" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.140625" style="13" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="4" max="6" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="13" width="24.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1450,6 +1465,9 @@
       <c r="G2" s="11" t="s">
         <v>81</v>
       </c>
+      <c r="H2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1467,6 +1485,9 @@
         <v>5</v>
       </c>
       <c r="G3" s="11"/>
+      <c r="H3" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1488,6 +1509,9 @@
         <v>31</v>
       </c>
       <c r="G4" s="11"/>
+      <c r="H4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -1511,6 +1535,9 @@
       <c r="G5" s="11" t="s">
         <v>33</v>
       </c>
+      <c r="H5" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -1534,6 +1561,9 @@
       <c r="G6" s="11" t="s">
         <v>34</v>
       </c>
+      <c r="H6" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -1555,6 +1585,9 @@
         <v>31</v>
       </c>
       <c r="G7" s="11"/>
+      <c r="H7" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1572,6 +1605,9 @@
         <v>6</v>
       </c>
       <c r="G8" s="11"/>
+      <c r="H8" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -1593,6 +1629,9 @@
         <v>31</v>
       </c>
       <c r="G9" s="11"/>
+      <c r="H9" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -1610,6 +1649,9 @@
         <v>7</v>
       </c>
       <c r="G10" s="11"/>
+      <c r="H10" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -1629,6 +1671,9 @@
       <c r="G11" s="12" t="s">
         <v>81</v>
       </c>
+      <c r="H11" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1646,6 +1691,9 @@
         <v>5</v>
       </c>
       <c r="G12" s="12"/>
+      <c r="H12" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -1667,6 +1715,9 @@
         <v>31</v>
       </c>
       <c r="G13" s="12"/>
+      <c r="H13" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -1690,6 +1741,9 @@
       <c r="G14" s="12" t="s">
         <v>48</v>
       </c>
+      <c r="H14" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -1713,6 +1767,9 @@
       <c r="G15" s="12" t="s">
         <v>34</v>
       </c>
+      <c r="H15" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -1734,8 +1791,11 @@
         <v>31</v>
       </c>
       <c r="G16" s="12"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
@@ -1751,8 +1811,11 @@
         <v>6</v>
       </c>
       <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>36</v>
       </c>
@@ -1774,8 +1837,11 @@
       <c r="G18" s="12" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>36</v>
       </c>
@@ -1791,8 +1857,11 @@
         <v>7</v>
       </c>
       <c r="G19" s="12"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>82</v>
       </c>
@@ -1810,8 +1879,11 @@
       <c r="G20" s="11" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>82</v>
       </c>
@@ -1827,8 +1899,11 @@
         <v>5</v>
       </c>
       <c r="G21" s="11"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>82</v>
       </c>
@@ -1848,8 +1923,11 @@
         <v>31</v>
       </c>
       <c r="G22" s="11"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>82</v>
       </c>
@@ -1871,8 +1949,11 @@
       <c r="G23" s="11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>82</v>
       </c>
@@ -1894,8 +1975,11 @@
       <c r="G24" s="11" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>82</v>
       </c>
@@ -1915,8 +1999,11 @@
         <v>31</v>
       </c>
       <c r="G25" s="11"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>82</v>
       </c>
@@ -1932,8 +2019,11 @@
         <v>6</v>
       </c>
       <c r="G26" s="11"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>82</v>
       </c>
@@ -1955,8 +2045,11 @@
       <c r="G27" s="11" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>82</v>
       </c>
@@ -1976,8 +2069,11 @@
         <v>103</v>
       </c>
       <c r="G28" s="11"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>82</v>
       </c>
@@ -1997,8 +2093,11 @@
         <v>31</v>
       </c>
       <c r="G29" s="11"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>82</v>
       </c>
@@ -2018,8 +2117,11 @@
         <v>31</v>
       </c>
       <c r="G30" s="11"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>82</v>
       </c>
@@ -2041,8 +2143,11 @@
       <c r="G31" s="18" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>82</v>
       </c>
@@ -2062,8 +2167,11 @@
         <v>105</v>
       </c>
       <c r="G32" s="11"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>82</v>
       </c>
@@ -2079,6 +2187,9 @@
         <v>7</v>
       </c>
       <c r="G33" s="11"/>
+      <c r="H33" t="s">
+        <v>110</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -2107,13 +2218,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="26" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>